<commit_message>
Update Query of intern
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49" count="49">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48" count="48">
   <x:si>
     <x:t>Id</x:t>
   </x:si>
@@ -55,16 +55,16 @@
     <x:t>jayeerythm8@gmail.com</x:t>
   </x:si>
   <x:si>
-    <x:t>Web developer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Frontend &amp; Backend</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2020-04-22T18:30:00.000Z</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2020-06-22T18:30:00.000Z</x:t>
+    <x:t> Web developer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Frontend &amp; </x:t>
+  </x:si>
+  <x:si>
+    <x:t>2020-06-02T18:30:00.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2020-06-15T18:30:00.000Z</x:t>
   </x:si>
   <x:si>
     <x:t>100000</x:t>
@@ -110,9 +110,6 @@
   </x:si>
   <x:si>
     <x:t>acfsdzvff@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2020-06-15T18:30:00.000Z</x:t>
   </x:si>
   <x:si>
     <x:t>2020-06-24T18:30:00.000Z</x:t>
@@ -680,19 +677,19 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G5" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="G5" s="0" t="s">
+      <x:c r="H5" s="0" t="s">
         <x:v>33</x:v>
-      </x:c>
-      <x:c r="H5" s="0" t="s">
-        <x:v>34</x:v>
       </x:c>
       <x:c r="I5" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
       <x:c r="J5" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="K5" s="0" t="s">
         <x:v>30</x:v>
@@ -715,19 +712,19 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="F6" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="G6" s="0" t="s">
+      <x:c r="H6" s="0" t="s">
         <x:v>33</x:v>
-      </x:c>
-      <x:c r="H6" s="0" t="s">
-        <x:v>34</x:v>
       </x:c>
       <x:c r="I6" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
       <x:c r="J6" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="K6" s="0" t="s">
         <x:v>30</x:v>
@@ -750,19 +747,19 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="F7" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G7" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="G7" s="0" t="s">
+      <x:c r="H7" s="0" t="s">
         <x:v>33</x:v>
-      </x:c>
-      <x:c r="H7" s="0" t="s">
-        <x:v>34</x:v>
       </x:c>
       <x:c r="I7" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
       <x:c r="J7" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="K7" s="0" t="s">
         <x:v>30</x:v>
@@ -785,22 +782,22 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="F8" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="G8" s="0" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="G8" s="0" t="s">
+      <x:c r="H8" s="0" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="H8" s="0" t="s">
+      <x:c r="I8" s="0" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="I8" s="0" t="s">
+      <x:c r="J8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K8" s="0" t="s">
         <x:v>40</x:v>
-      </x:c>
-      <x:c r="J8" s="0" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="K8" s="0" t="s">
-        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:11">
@@ -820,22 +817,22 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="F9" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="G9" s="0" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="G9" s="0" t="s">
+      <x:c r="H9" s="0" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="H9" s="0" t="s">
+      <x:c r="I9" s="0" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="I9" s="0" t="s">
+      <x:c r="J9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K9" s="0" t="s">
         <x:v>40</x:v>
-      </x:c>
-      <x:c r="J9" s="0" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="K9" s="0" t="s">
-        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:11">
@@ -855,19 +852,19 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="F10" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="G10" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="H10" s="0" t="s">
         <x:v>42</x:v>
-      </x:c>
-      <x:c r="H10" s="0" t="s">
-        <x:v>43</x:v>
       </x:c>
       <x:c r="I10" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
       <x:c r="J10" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="K10" s="0" t="s">
         <x:v>30</x:v>
@@ -878,34 +875,34 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="F11" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="H11" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="I11" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="J11" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="K11" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:11">
@@ -913,34 +910,34 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="F12" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="H12" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="I12" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="J12" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="K12" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:11">
@@ -948,34 +945,34 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="F13" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G13" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="H13" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="I13" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="J13" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="K13" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:11">
@@ -983,34 +980,34 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="E14" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="F14" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G14" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="H14" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="I14" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="J14" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="K14" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:11">
@@ -1018,34 +1015,34 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="E15" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="F15" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G15" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="H15" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="I15" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="J15" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="K15" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:11">
@@ -1053,34 +1050,34 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="E16" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="F16" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G16" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="H16" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="I16" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="J16" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="K16" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:11">
@@ -1088,34 +1085,34 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="E17" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="F17" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G17" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="H17" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="I17" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="J17" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="K17" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:11">
@@ -1123,34 +1120,34 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="E18" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="F18" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G18" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="H18" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="I18" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="J18" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="K18" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:11">
@@ -1158,34 +1155,34 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="E19" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="F19" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G19" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="H19" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="I19" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="J19" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="K19" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:11">
@@ -1193,7 +1190,7 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
         <x:v>31</x:v>
@@ -1208,16 +1205,16 @@
         <x:v>25</x:v>
       </x:c>
       <x:c r="G20" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="H20" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="H20" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
       <x:c r="I20" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="J20" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="K20" s="0" t="s">
         <x:v>30</x:v>
@@ -1228,34 +1225,34 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="E21" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="F21" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G21" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="H21" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="I21" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="J21" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="K21" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Delete Intern from the table
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -109,55 +109,10 @@
     <x:t>sfwewefsvds</x:t>
   </x:si>
   <x:si>
-    <x:t>acfsdzvff@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2020-06-24T18:30:00.000Z</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12312</x:t>
-  </x:si>
-  <x:si>
-    <x:t>867sdfds</x:t>
-  </x:si>
-  <x:si>
-    <x:t>867sdfdssd</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2020-06-06T18:30:00.000Z</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2020-06-23T18:30:00.000Z</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7889</x:t>
-  </x:si>
-  <x:si>
-    <x:t>dsfsfsdsf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>sdfgewadasfsdf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2020-06-19T18:30:00.000Z</x:t>
-  </x:si>
-  <x:si>
-    <x:t>77777</x:t>
-  </x:si>
-  <x:si>
     <x:t/>
   </x:si>
   <x:si>
     <x:t>0000-00-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>kdfjhsik</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2020-06-30T18:30:00.000Z</x:t>
-  </x:si>
-  <x:si>
-    <x:t>87878</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -662,597 +617,352 @@
     </x:row>
     <x:row r="5" spans="1:11">
       <x:c r="A5" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
         <x:v>31</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G5" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
       <x:c r="H5" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="I5" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="J5" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="K5" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:11">
       <x:c r="A6" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
         <x:v>31</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="F6" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G6" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
       <x:c r="H6" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="I6" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="J6" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="K6" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:11">
       <x:c r="A7" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
         <x:v>31</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="F7" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G7" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
       <x:c r="H7" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="I7" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="J7" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="K7" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:11">
       <x:c r="A8" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
         <x:v>31</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="F8" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G8" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="H8" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="I8" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="J8" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="K8" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:11">
       <x:c r="A9" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
         <x:v>31</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="F9" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G9" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="H9" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="I9" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="J9" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="K9" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:11">
       <x:c r="A10" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
         <x:v>31</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="F10" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G10" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="H10" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="I10" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="J10" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="K10" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:11">
       <x:c r="A11" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="F11" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="H11" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="I11" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="J11" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="K11" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:11">
       <x:c r="A12" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="F12" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="H12" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="I12" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="J12" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="K12" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:11">
       <x:c r="A13" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="F13" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G13" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="H13" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="I13" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="J13" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="K13" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:11">
       <x:c r="A14" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="E14" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="F14" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G14" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="H14" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="I14" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="J14" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="K14" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:11">
-      <x:c r="A15" s="0" t="n">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="B15" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="C15" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="D15" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="E15" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="F15" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="G15" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="H15" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="I15" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="J15" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="K15" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:11">
-      <x:c r="A16" s="0" t="n">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="B16" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="C16" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="D16" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="E16" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="F16" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="G16" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="H16" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="I16" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="J16" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="K16" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:11">
-      <x:c r="A17" s="0" t="n">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="B17" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="C17" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="D17" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="E17" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="F17" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="G17" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="H17" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="I17" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="J17" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="K17" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:11">
-      <x:c r="A18" s="0" t="n">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="B18" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="C18" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="D18" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="E18" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="F18" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="G18" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="H18" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="I18" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="J18" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="K18" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:11">
-      <x:c r="A19" s="0" t="n">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="B19" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="C19" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="D19" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="E19" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="F19" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="G19" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="H19" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="I19" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="J19" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="K19" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:11">
-      <x:c r="A20" s="0" t="n">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="B20" s="0" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="C20" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="D20" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="E20" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="F20" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="G20" s="0" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="H20" s="0" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="I20" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="J20" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="K20" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:11">
-      <x:c r="A21" s="0" t="n">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="B21" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="C21" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="D21" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="E21" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="F21" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="G21" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="H21" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="I21" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="J21" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="K21" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>